<commit_message>
added EDA related to sentiment
</commit_message>
<xml_diff>
--- a/movie_sentiment/output/result_for_report.xlsx
+++ b/movie_sentiment/output/result_for_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ceffendy\Documents\GitHub\KM6312_MovieReviewSentiment\movie_sentiment\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCACEBA-CA37-4CC4-88CB-C73ADF7746D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE295E1-3F87-4E7D-86CA-F0EA1ED6D71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{22DC5596-5AAE-4999-9E9F-6A9339BEFA68}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" activeTab="4" xr2:uid="{22DC5596-5AAE-4999-9E9F-6A9339BEFA68}"/>
   </bookViews>
   <sheets>
     <sheet name="LR" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="25">
   <si>
     <t>C</t>
   </si>
@@ -192,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -223,15 +223,26 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -568,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1803F952-A1CF-4CC0-8FD7-890E03446DB8}">
-  <dimension ref="B1:H8"/>
+  <dimension ref="B1:H7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,49 +623,49 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>100000</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.74403056351480401</v>
-      </c>
-      <c r="H3" s="13">
-        <v>5.7127451896667401</v>
+      <c r="F3" s="2">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.77459407831900595</v>
+      </c>
+      <c r="H3" s="14">
+        <v>1.4211678504943801</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
-        <v>100000</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.75549188156638003</v>
-      </c>
-      <c r="H4" s="13">
-        <v>0.18220686912536599</v>
+      <c r="B4" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20">
+        <v>6</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="20">
+        <v>3</v>
+      </c>
+      <c r="F4" s="20">
+        <v>100000</v>
+      </c>
+      <c r="G4" s="21">
+        <v>0.768863419293218</v>
+      </c>
+      <c r="H4" s="22">
+        <v>4.6005957126617396</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -662,104 +673,84 @@
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.76408787010506196</v>
+      </c>
+      <c r="H5" s="13">
+        <v>16.841151475906301</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
         <v>2</v>
       </c>
-      <c r="F5" s="1">
-        <v>100000</v>
-      </c>
-      <c r="G5" s="4">
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G6" s="4">
         <v>0.75549188156638003</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H6" s="13">
+        <v>0.18220686912536599</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
+        <v>3</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="6">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6">
+        <v>100000</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0.75549188156638003</v>
+      </c>
+      <c r="H7" s="15">
         <v>8.0196323394775302</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>4</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2">
-        <v>2</v>
-      </c>
-      <c r="F6" s="2">
-        <v>100000</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0.77459407831900595</v>
-      </c>
-      <c r="H6" s="14">
-        <v>1.4211678504943801</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1">
-        <v>3</v>
-      </c>
-      <c r="F7" s="1">
-        <v>100000</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0.76408787010506196</v>
-      </c>
-      <c r="H7" s="13">
-        <v>16.841151475906301</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6">
-        <v>6</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="6">
-        <v>3</v>
-      </c>
-      <c r="F8" s="6">
-        <v>100000</v>
-      </c>
-      <c r="G8" s="7">
-        <v>0.768863419293218</v>
-      </c>
-      <c r="H8" s="15">
-        <v>4.6005957126617396</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:H7">
+    <sortCondition descending="1" ref="G3:G7"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DFC32CD-738F-4ACF-83C5-87FDD0D6475B}">
-  <dimension ref="B1:H8"/>
+  <dimension ref="B1:H7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H2"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,26 +791,26 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>100000</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.71442215854823299</v>
-      </c>
-      <c r="H3" s="3">
-        <v>6.5813753604888898</v>
+      <c r="C3" s="23">
+        <v>6</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="23">
+        <v>3</v>
+      </c>
+      <c r="F3" s="23">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="24">
+        <v>0.77841451766953196</v>
+      </c>
+      <c r="H3" s="25">
+        <v>1.11026883125305</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -827,22 +818,22 @@
         <v>4</v>
       </c>
       <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
       <c r="F4" s="1">
         <v>100000</v>
       </c>
       <c r="G4" s="4">
-        <v>0.73447946513849005</v>
+        <v>0.77363896848137503</v>
       </c>
       <c r="H4" s="3">
-        <v>0.24589562416076599</v>
+        <v>0.43312954902648898</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -850,94 +841,74 @@
         <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0.73447946513849005</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.24589562416076599</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="20">
+        <v>3</v>
+      </c>
+      <c r="D6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E6" s="20">
         <v>2</v>
       </c>
-      <c r="F5" s="1">
-        <v>100000</v>
-      </c>
-      <c r="G5" s="4">
+      <c r="F6" s="20">
+        <v>100000</v>
+      </c>
+      <c r="G6" s="21">
         <v>0.73161413562559696</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H6" s="26">
         <v>25.822370290756201</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="C7" s="6">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="1">
-        <v>100000</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0.77363896848137503</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.43312954902648898</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1">
-        <v>3</v>
-      </c>
-      <c r="F7" s="1">
-        <v>100000</v>
-      </c>
-      <c r="G7" s="4">
+      <c r="E7" s="6">
+        <v>3</v>
+      </c>
+      <c r="F7" s="6">
+        <v>100000</v>
+      </c>
+      <c r="G7" s="7">
         <v>0.72779369627507096</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="8">
         <v>57.951539516448896</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="16">
-        <v>6</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="16">
-        <v>3</v>
-      </c>
-      <c r="F8" s="16">
-        <v>100000</v>
-      </c>
-      <c r="G8" s="17">
-        <v>0.77841451766953196</v>
-      </c>
-      <c r="H8" s="18">
-        <v>1.11026883125305</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:H7">
+    <sortCondition descending="1" ref="G3:G7"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -947,7 +918,7 @@
   <dimension ref="B1:J7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,7 +929,7 @@
     <col min="4" max="4" width="6.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" style="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -982,7 +953,7 @@
       <c r="F2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="11" t="s">
@@ -996,31 +967,31 @@
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>21</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
         <v>2</v>
       </c>
-      <c r="F3" s="1">
-        <v>100000</v>
-      </c>
-      <c r="G3" s="19">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="F3" s="2">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="27">
+        <v>1</v>
+      </c>
+      <c r="H3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="5">
         <v>0.76313276026743004</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="28">
         <v>197.56319808959901</v>
       </c>
     </row>
@@ -1040,7 +1011,7 @@
       <c r="F4" s="1">
         <v>100000</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="16">
         <v>1</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -1069,7 +1040,7 @@
       <c r="F5" s="1">
         <v>100000</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="16">
         <v>100</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -1098,7 +1069,7 @@
       <c r="F6" s="1">
         <v>100000</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="16">
         <v>1</v>
       </c>
       <c r="H6" s="3" t="s">
@@ -1127,7 +1098,7 @@
       <c r="F7" s="6">
         <v>100000</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="18">
         <v>100</v>
       </c>
       <c r="H7" s="8" t="s">
@@ -1141,6 +1112,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:J7">
+    <sortCondition descending="1" ref="I3:I7"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1149,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845C75AC-7730-4960-B8BE-78F040977D16}">
   <dimension ref="B1:K7"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,8 +1136,8 @@
     <col min="5" max="5" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" style="19" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" style="19" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" style="16" customWidth="1"/>
+    <col min="9" max="9" width="4.28515625" style="16" customWidth="1"/>
     <col min="10" max="10" width="7.5703125" style="4" customWidth="1"/>
     <col min="11" max="11" width="8.42578125" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
@@ -1189,10 +1163,10 @@
       <c r="G2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="17" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="10" t="s">
@@ -1203,34 +1177,34 @@
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="5">
         <v>0.66380133715377199</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="28">
         <v>6.1156647205352703</v>
       </c>
     </row>
@@ -1253,10 +1227,10 @@
       <c r="G4" s="1">
         <v>10</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="16">
         <v>20</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="16">
         <v>20</v>
       </c>
       <c r="J4" s="4">
@@ -1282,13 +1256,13 @@
       <c r="F5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="19" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="4">
@@ -1314,13 +1288,13 @@
       <c r="F6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="19" t="s">
         <v>23</v>
       </c>
       <c r="J6" s="4">
@@ -1349,10 +1323,10 @@
       <c r="G7" s="6">
         <v>10</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="18">
         <v>20</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="18">
         <v>20</v>
       </c>
       <c r="J7" s="7">
@@ -1371,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{766300AC-A23B-439C-94CC-10586ED209F8}">
   <dimension ref="B1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,25 +1387,25 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>100000</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="5">
         <v>0.73664122137404497</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="28">
         <v>209.15093350410399</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EL, BERT, Inference, app updates
</commit_message>
<xml_diff>
--- a/movie_sentiment/output/result_for_report.xlsx
+++ b/movie_sentiment/output/result_for_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ceffendy\Documents\GitHub\KM6312_MovieReviewSentiment\movie_sentiment\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60ED0F43-836A-49E1-BC0A-D6C2435B24CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA87D02-9A7A-4A52-A4DC-7326ABF767D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{22DC5596-5AAE-4999-9E9F-6A9339BEFA68}"/>
+    <workbookView xWindow="1905" yWindow="2220" windowWidth="21600" windowHeight="11235" activeTab="5" xr2:uid="{22DC5596-5AAE-4999-9E9F-6A9339BEFA68}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="6" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="DT" sheetId="4" r:id="rId5"/>
     <sheet name="EL" sheetId="5" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="socher" localSheetId="5">EL!$B$3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="42">
   <si>
     <t>C</t>
   </si>
@@ -115,9 +118,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Stack</t>
-  </si>
-  <si>
     <t>distilbert-base-uncased-finetuned-sst-2-english</t>
   </si>
   <si>
@@ -130,9 +130,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>learning rate:2e-5, batch:16, number of epoch:3, weight decay: 0.01</t>
-  </si>
-  <si>
     <t>Remarks</t>
   </si>
   <si>
@@ -145,19 +142,10 @@
     <t>18 models</t>
   </si>
   <si>
-    <t>3 models</t>
-  </si>
-  <si>
     <t>36 models</t>
   </si>
   <si>
-    <t>70 models</t>
-  </si>
-  <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Ensemble</t>
   </si>
   <si>
     <t>The best model: Ensemble - 1, text_preprocess: True, vectorizer: tfidf, ngram: 1, max_iter: 100000
@@ -172,6 +160,18 @@
   </si>
   <si>
     <t>LR, RBF, DT</t>
+  </si>
+  <si>
+    <t>learning rate:2e-5, batch:16, number of epoch:3, weight decay: 0.01, max_length=256</t>
+  </si>
+  <si>
+    <t>Ensemble (LR, RBF, DT)</t>
+  </si>
+  <si>
+    <t>73 models</t>
+  </si>
+  <si>
+    <t>Ensemble  (LR, SVM LR, RBF, DT)</t>
   </si>
 </sst>
 </file>
@@ -298,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -368,9 +368,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -402,53 +399,58 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -789,28 +791,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C237E5-B048-4805-B6AC-148598D20666}">
-  <dimension ref="B1:O20"/>
+  <dimension ref="B1:O21"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.28515625" style="37" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" style="36" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" style="46" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" style="58" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="45" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" style="48" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -851,15 +853,15 @@
       <c r="M2" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="36" t="s">
+      <c r="N2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="57" t="s">
-        <v>30</v>
+      <c r="O2" s="47" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:15" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="37" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="23">
@@ -892,14 +894,14 @@
       <c r="L3" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="47">
+      <c r="M3" s="52">
         <v>0.77459407831900595</v>
       </c>
       <c r="N3" s="25">
         <v>0.91207957267761197</v>
       </c>
-      <c r="O3" s="62" t="s">
-        <v>31</v>
+      <c r="O3" s="66" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
@@ -936,16 +938,16 @@
       <c r="L4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="48">
+      <c r="M4" s="53">
         <v>0.768863419293218</v>
       </c>
       <c r="N4" s="13">
         <v>3.0163316726684499</v>
       </c>
-      <c r="O4" s="63"/>
+      <c r="O4" s="67"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="38" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="6">
@@ -978,16 +980,16 @@
       <c r="L5" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="49">
+      <c r="M5" s="54">
         <v>0.76408787010506196</v>
       </c>
       <c r="N5" s="14">
         <v>10.8985826969146</v>
       </c>
-      <c r="O5" s="64"/>
+      <c r="O5" s="68"/>
     </row>
     <row r="6" spans="2:15" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="39" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="27">
@@ -1020,14 +1022,14 @@
       <c r="L6" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="M6" s="50">
+      <c r="M6" s="55">
         <v>0.77841451766953196</v>
       </c>
       <c r="N6" s="29">
         <v>0.64355731010437001</v>
       </c>
-      <c r="O6" s="62" t="s">
-        <v>31</v>
+      <c r="O6" s="66" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -1064,16 +1066,16 @@
       <c r="L7" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="48">
+      <c r="M7" s="53">
         <v>0.77363896848137503</v>
       </c>
       <c r="N7" s="3">
         <v>0.333178520202636</v>
       </c>
-      <c r="O7" s="63"/>
+      <c r="O7" s="67"/>
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="38" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="6">
@@ -1106,16 +1108,16 @@
       <c r="L8" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="M8" s="49">
+      <c r="M8" s="54">
         <v>0.73447946513849005</v>
       </c>
       <c r="N8" s="8">
         <v>0.17733573913574199</v>
       </c>
-      <c r="O8" s="64"/>
+      <c r="O8" s="68"/>
     </row>
     <row r="9" spans="2:15" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="39" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="27">
@@ -1148,14 +1150,14 @@
       <c r="L9" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="M9" s="50">
+      <c r="M9" s="55">
         <v>0.76313276026743004</v>
       </c>
       <c r="N9" s="29">
         <v>318.744499206542</v>
       </c>
-      <c r="O9" s="62" t="s">
-        <v>35</v>
+      <c r="O9" s="66" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -1192,16 +1194,16 @@
       <c r="L10" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="M10" s="48">
+      <c r="M10" s="53">
         <v>0.76217765042979901</v>
       </c>
       <c r="N10" s="3">
         <v>73.361222982406602</v>
       </c>
-      <c r="O10" s="63"/>
+      <c r="O10" s="67"/>
     </row>
     <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="6">
@@ -1234,16 +1236,16 @@
       <c r="L11" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="49">
+      <c r="M11" s="54">
         <v>0.76026743075453596</v>
       </c>
       <c r="N11" s="8">
         <v>480.84639716148303</v>
       </c>
-      <c r="O11" s="64"/>
+      <c r="O11" s="68"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="39" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="27">
@@ -1276,14 +1278,14 @@
       <c r="L12" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="50">
+      <c r="M12" s="55">
         <v>0.66380133715377199</v>
       </c>
       <c r="N12" s="29">
         <v>14.915147781371999</v>
       </c>
-      <c r="O12" s="62" t="s">
-        <v>33</v>
+      <c r="O12" s="66" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
@@ -1320,16 +1322,16 @@
       <c r="L13" s="15">
         <v>20</v>
       </c>
-      <c r="M13" s="48">
+      <c r="M13" s="53">
         <v>0.66380133715377199</v>
       </c>
       <c r="N13" s="3">
         <v>11.0135858058929</v>
       </c>
-      <c r="O13" s="63"/>
+      <c r="O13" s="67"/>
     </row>
     <row r="14" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="38" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="6">
@@ -1362,17 +1364,17 @@
       <c r="L14" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="M14" s="49">
+      <c r="M14" s="54">
         <v>0.66380133715377199</v>
       </c>
       <c r="N14" s="8">
         <v>12.2938024997711</v>
       </c>
-      <c r="O14" s="64"/>
+      <c r="O14" s="68"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="41" t="s">
-        <v>38</v>
+      <c r="B15" s="40" t="s">
+        <v>39</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
@@ -1404,70 +1406,70 @@
       <c r="L15" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="M15" s="5">
-        <v>0.73664122137404497</v>
+      <c r="M15" s="57">
+        <v>0.73638968500000002</v>
       </c>
       <c r="N15" s="18">
-        <v>209.15093350410399</v>
-      </c>
-      <c r="O15" s="62" t="s">
-        <v>34</v>
+        <v>128.005053</v>
+      </c>
+      <c r="O15" s="66" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16" s="53">
+        <v>0.71442215899999995</v>
+      </c>
+      <c r="N16" s="3">
+        <v>68.13478112</v>
+      </c>
+      <c r="O16" s="67"/>
+    </row>
+    <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="6">
         <v>2</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-      <c r="F16" s="1">
-        <v>100000</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="L16" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="M16" s="4">
-        <v>0.711832061068702</v>
-      </c>
-      <c r="N16" s="3">
-        <v>714.28744220733597</v>
-      </c>
-      <c r="O16" s="63"/>
-    </row>
-    <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="6">
-        <v>3</v>
-      </c>
       <c r="D17" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F17" s="6">
         <v>100000</v>
@@ -1490,13 +1492,13 @@
       <c r="L17" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="7">
-        <v>0.69465648854961803</v>
+      <c r="M17" s="54">
+        <v>0.70200573099999997</v>
       </c>
       <c r="N17" s="8">
-        <v>1443.15357303619</v>
-      </c>
-      <c r="O17" s="64"/>
+        <v>573.00046680000003</v>
+      </c>
+      <c r="O17" s="68"/>
     </row>
     <row r="18" spans="2:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="34" t="s">
@@ -1508,75 +1510,91 @@
       <c r="D18" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="61" t="s">
+      <c r="E18" s="65" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="65"/>
+      <c r="N18" s="65"/>
+      <c r="O18" s="34"/>
+    </row>
+    <row r="19" spans="2:15" s="41" customFormat="1" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="43">
+        <v>1</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="56">
+        <v>0.91969407299999995</v>
+      </c>
+      <c r="N19" s="46">
+        <v>239.96809999999999</v>
+      </c>
+      <c r="O19" s="49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="12"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="61"/>
-      <c r="L18" s="61"/>
-      <c r="M18" s="61"/>
-      <c r="N18" s="61"/>
-      <c r="O18" s="34"/>
-    </row>
-    <row r="19" spans="2:15" s="42" customFormat="1" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="44">
-        <v>1</v>
-      </c>
-      <c r="D19" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="52" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="53">
-        <v>0.93879999999999997</v>
-      </c>
-      <c r="N19" s="54">
-        <f>14348.7688+100.0609</f>
-        <v>14448.8297</v>
-      </c>
-      <c r="O19" s="59" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="55"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="51"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51"/>
-      <c r="N20" s="60" t="s">
-        <v>37</v>
-      </c>
-      <c r="O20" s="56" t="s">
-        <v>36</v>
-      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="O20" s="63" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="58"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="60"/>
+      <c r="N21" s="60"/>
+      <c r="O21" s="61"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="E19:L19"/>
     <mergeCell ref="E18:N18"/>
     <mergeCell ref="O3:O5"/>
     <mergeCell ref="O6:O8"/>
@@ -1837,7 +1855,7 @@
   <dimension ref="B1:J5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J5"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2143,14 +2161,14 @@
   <dimension ref="B1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -2187,7 +2205,7 @@
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -2202,18 +2220,18 @@
         <v>100000</v>
       </c>
       <c r="G3" s="5">
-        <v>0.73664122137404497</v>
+        <v>0.73638968500000002</v>
       </c>
       <c r="H3" s="18">
-        <v>209.15093350410399</v>
+        <v>128.005053</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
@@ -2225,53 +2243,53 @@
         <v>100000</v>
       </c>
       <c r="G4" s="4">
-        <v>0.711832061068702</v>
+        <v>0.71442215899999995</v>
       </c>
       <c r="H4" s="3">
-        <v>714.28744220733597</v>
+        <v>68.13478112</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C5" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5" s="6">
         <v>100000</v>
       </c>
       <c r="G5" s="7">
-        <v>0.69465648854961803</v>
+        <v>0.70200573099999997</v>
       </c>
       <c r="H5" s="8">
-        <v>1443.15357303619</v>
+        <v>573.00046680000003</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J6" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="J7" s="12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J9" s="66" t="s">
-        <v>42</v>
+      <c r="J9" s="51" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="J10" s="65" t="s">
-        <v>41</v>
+      <c r="J10" s="50" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update walltime for bert
</commit_message>
<xml_diff>
--- a/movie_sentiment/output/result_for_report.xlsx
+++ b/movie_sentiment/output/result_for_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ceffendy\Documents\GitHub\KM6312_MovieReviewSentiment\movie_sentiment\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42534A8B-2E51-4AAD-8E85-4E23AE0E3D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B356B886-AB07-4DF1-B93D-8F1A419198B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{22DC5596-5AAE-4999-9E9F-6A9339BEFA68}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22DC5596-5AAE-4999-9E9F-6A9339BEFA68}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="6" r:id="rId1"/>
@@ -217,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -268,17 +268,28 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -319,9 +330,6 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -329,19 +337,7 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -357,39 +353,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -403,25 +375,74 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -764,13 +785,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C237E5-B048-4805-B6AC-148598D20666}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.42578125" style="36" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" style="29" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
@@ -781,805 +802,805 @@
     <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="45" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" style="45" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" style="48" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" style="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="51"/>
+      <c r="A1" s="36"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="36"/>
     </row>
     <row r="2" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="34" t="s">
+      <c r="A2" s="36"/>
+      <c r="B2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="N2" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="47" t="s">
+      <c r="O2" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="51"/>
-    </row>
-    <row r="3" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62"/>
-      <c r="B3" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="23">
+      <c r="P2" s="36"/>
+    </row>
+    <row r="3" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="42"/>
+      <c r="B3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="22">
         <v>4</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="23">
+      <c r="D3" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="22">
         <v>2</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="22">
         <v>100000</v>
       </c>
-      <c r="G3" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="61">
+      <c r="G3" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="41">
         <v>0.77459407831900595</v>
       </c>
-      <c r="N3" s="25">
+      <c r="N3" s="24">
         <v>0.91207957267761197</v>
       </c>
-      <c r="O3" s="58" t="s">
+      <c r="O3" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="62"/>
+      <c r="P3" s="42"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
-      <c r="B4" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="A4" s="36"/>
+      <c r="B4" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="48">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="D4" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="48">
+        <v>3</v>
+      </c>
+      <c r="F4" s="48">
         <v>100000</v>
       </c>
-      <c r="G4" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" s="3">
+      <c r="G4" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="49">
         <v>0.768863419293218</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="50">
         <v>3.0163316726684499</v>
       </c>
-      <c r="O4" s="59"/>
-      <c r="P4" s="51"/>
-    </row>
-    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
-      <c r="B5" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="O4" s="46"/>
+      <c r="P4" s="36"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="36"/>
+      <c r="B5" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="52">
         <v>5</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="6">
-        <v>3</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="E5" s="52">
+        <v>3</v>
+      </c>
+      <c r="F5" s="52">
         <v>100000</v>
       </c>
-      <c r="G5" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="8">
+      <c r="G5" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="54">
         <v>0.76408787010506196</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="55">
         <v>10.8985826969146</v>
       </c>
-      <c r="O5" s="60"/>
-      <c r="P5" s="51"/>
-    </row>
-    <row r="6" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
-      <c r="B6" s="39" t="s">
+      <c r="O5" s="56"/>
+      <c r="P5" s="36"/>
+    </row>
+    <row r="6" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="42"/>
+      <c r="B6" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="22">
         <v>6</v>
       </c>
-      <c r="D6" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="27">
-        <v>3</v>
-      </c>
-      <c r="F6" s="27">
+      <c r="D6" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="22">
+        <v>3</v>
+      </c>
+      <c r="F6" s="22">
         <v>100000</v>
       </c>
-      <c r="G6" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" s="29">
+      <c r="G6" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="41">
         <v>0.77841451766953196</v>
       </c>
-      <c r="N6" s="29">
+      <c r="N6" s="41">
         <v>0.64355731010437001</v>
       </c>
-      <c r="O6" s="58" t="s">
+      <c r="O6" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="62"/>
+      <c r="P6" s="42"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="36"/>
+      <c r="B7" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="48">
         <v>4</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="D7" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="48">
         <v>2</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="48">
         <v>100000</v>
       </c>
-      <c r="G7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="M7" s="3">
+      <c r="G7" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="49">
         <v>0.77363896848137503</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="49">
         <v>0.333178520202636</v>
       </c>
-      <c r="O7" s="59"/>
-      <c r="P7" s="51"/>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="51"/>
-      <c r="B8" s="38" t="s">
+      <c r="O7" s="46"/>
+      <c r="P7" s="36"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="36"/>
+      <c r="B8" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="52">
         <v>2</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1</v>
-      </c>
-      <c r="F8" s="6">
+      <c r="D8" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="52">
+        <v>1</v>
+      </c>
+      <c r="F8" s="52">
         <v>100000</v>
       </c>
-      <c r="G8" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" s="8">
+      <c r="G8" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="54">
         <v>0.73447946513849005</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="54">
         <v>0.17733573913574199</v>
       </c>
-      <c r="O8" s="60"/>
-      <c r="P8" s="51"/>
-    </row>
-    <row r="9" spans="1:16" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
-      <c r="B9" s="39" t="s">
+      <c r="O8" s="56"/>
+      <c r="P8" s="36"/>
+    </row>
+    <row r="9" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="42"/>
+      <c r="B9" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="22">
         <v>21</v>
       </c>
-      <c r="D9" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="27">
+      <c r="D9" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="22">
         <v>2</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="22">
         <v>100000</v>
       </c>
-      <c r="G9" s="31">
-        <v>1</v>
-      </c>
-      <c r="H9" s="29" t="s">
+      <c r="G9" s="57">
+        <v>1</v>
+      </c>
+      <c r="H9" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="29">
+      <c r="I9" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="41">
         <v>0.76313276026743004</v>
       </c>
-      <c r="N9" s="29">
+      <c r="N9" s="41">
         <v>318.744499206542</v>
       </c>
-      <c r="O9" s="58" t="s">
+      <c r="O9" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="P9" s="62"/>
+      <c r="P9" s="42"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="36"/>
+      <c r="B10" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="48">
         <v>9</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="D10" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="48">
+        <v>1</v>
+      </c>
+      <c r="F10" s="48">
         <v>100000</v>
       </c>
-      <c r="G10" s="15">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="G10" s="58">
+        <v>1</v>
+      </c>
+      <c r="H10" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="3">
+      <c r="I10" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="49">
         <v>0.76217765042979901</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="49">
         <v>73.361222982406602</v>
       </c>
-      <c r="O10" s="59"/>
-      <c r="P10" s="51"/>
-    </row>
-    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="51"/>
-      <c r="B11" s="38" t="s">
+      <c r="O10" s="46"/>
+      <c r="P10" s="36"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="36"/>
+      <c r="B11" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="6">
-        <v>23</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="C11" s="52">
+        <v>23</v>
+      </c>
+      <c r="D11" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="52">
         <v>2</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="52">
         <v>100000</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="59">
         <v>100</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="M11" s="8">
+      <c r="I11" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="54">
         <v>0.76026743075453596</v>
       </c>
-      <c r="N11" s="8">
+      <c r="N11" s="54">
         <v>480.84639716148303</v>
       </c>
-      <c r="O11" s="60"/>
-      <c r="P11" s="51"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="36"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
-      <c r="B12" s="39" t="s">
+      <c r="A12" s="36"/>
+      <c r="B12" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="22">
         <v>4</v>
       </c>
-      <c r="D12" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="27">
-        <v>1</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="27" t="s">
+      <c r="D12" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="22">
+        <v>1</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="M12" s="29">
+      <c r="J12" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="41">
         <v>0.66380133715377199</v>
       </c>
-      <c r="N12" s="29">
+      <c r="N12" s="41">
         <v>14.915147781371999</v>
       </c>
-      <c r="O12" s="58" t="s">
+      <c r="O12" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="P12" s="51"/>
+      <c r="P12" s="36"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="36"/>
+      <c r="B13" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="48">
         <v>5</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="D13" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="48">
+        <v>1</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="48">
         <v>10</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="58">
         <v>20</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="58">
         <v>20</v>
       </c>
-      <c r="M13" s="3">
+      <c r="M13" s="49">
         <v>0.66380133715377199</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="49">
         <v>11.0135858058929</v>
       </c>
-      <c r="O13" s="59"/>
-      <c r="P13" s="51"/>
-    </row>
-    <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="51"/>
-      <c r="B14" s="38" t="s">
+      <c r="O13" s="46"/>
+      <c r="P13" s="36"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="36"/>
+      <c r="B14" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="52">
         <v>6</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="H14" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="6" t="s">
+      <c r="D14" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="52">
+        <v>1</v>
+      </c>
+      <c r="F14" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="L14" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="M14" s="8">
+      <c r="J14" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" s="54">
         <v>0.66380133715377199</v>
       </c>
-      <c r="N14" s="8">
+      <c r="N14" s="54">
         <v>12.2938024997711</v>
       </c>
-      <c r="O14" s="60"/>
-      <c r="P14" s="51"/>
+      <c r="O14" s="56"/>
+      <c r="P14" s="36"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
-      <c r="B15" s="40" t="s">
+      <c r="A15" s="36"/>
+      <c r="B15" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="C15" s="22">
+        <v>1</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="22">
+        <v>1</v>
+      </c>
+      <c r="F15" s="22">
         <v>100000</v>
       </c>
-      <c r="G15" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="18">
+      <c r="G15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="41">
         <v>0.73638968500000002</v>
       </c>
-      <c r="N15" s="18">
+      <c r="N15" s="41">
         <v>128.005053</v>
       </c>
-      <c r="O15" s="58" t="s">
+      <c r="O15" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="P15" s="51"/>
+      <c r="P15" s="36"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
-      <c r="B16" s="12" t="s">
+      <c r="A16" s="36"/>
+      <c r="B16" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-      <c r="F16" s="1">
+      <c r="C16" s="48">
+        <v>1</v>
+      </c>
+      <c r="D16" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="48">
+        <v>1</v>
+      </c>
+      <c r="F16" s="48">
         <v>100000</v>
       </c>
-      <c r="G16" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="H16" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="L16" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="M16" s="3">
+      <c r="G16" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="J16" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16" s="49">
         <v>0.71442215899999995</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16" s="49">
         <v>68.13478112</v>
       </c>
-      <c r="O16" s="59"/>
-      <c r="P16" s="51"/>
-    </row>
-    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="51"/>
-      <c r="B17" s="38" t="s">
+      <c r="O16" s="46"/>
+      <c r="P16" s="36"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
+      <c r="B17" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="52">
         <v>2</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="6">
+      <c r="D17" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="52">
         <v>2</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="52">
         <v>100000</v>
       </c>
-      <c r="G17" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="L17" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="M17" s="8">
+      <c r="G17" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" s="54">
         <v>0.70200573099999997</v>
       </c>
-      <c r="N17" s="8">
+      <c r="N17" s="54">
         <v>573.00046680000003</v>
       </c>
-      <c r="O17" s="60"/>
-      <c r="P17" s="51"/>
-    </row>
-    <row r="18" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="51"/>
-      <c r="B18" s="34" t="s">
+      <c r="O17" s="56"/>
+      <c r="P17" s="36"/>
+    </row>
+    <row r="18" spans="1:16" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
+      <c r="B18" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="57" t="s">
+      <c r="E18" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="57"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="51"/>
-    </row>
-    <row r="19" spans="1:16" s="41" customFormat="1" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="63"/>
-      <c r="B19" s="42" t="s">
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69"/>
+      <c r="O18" s="68"/>
+      <c r="P18" s="36"/>
+    </row>
+    <row r="19" spans="1:16" s="31" customFormat="1" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="43"/>
+      <c r="B19" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="43">
-        <v>1</v>
-      </c>
-      <c r="D19" s="44" t="s">
+      <c r="C19" s="63">
+        <v>1</v>
+      </c>
+      <c r="D19" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="56" t="s">
+      <c r="E19" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
-      <c r="M19" s="46">
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="65"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="65"/>
+      <c r="M19" s="66">
         <v>0.91969407299999995</v>
       </c>
-      <c r="N19" s="46">
-        <v>239.96809999999999</v>
-      </c>
-      <c r="O19" s="49" t="s">
+      <c r="N19" s="66">
+        <v>14609.610408782901</v>
+      </c>
+      <c r="O19" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="P19" s="63"/>
+      <c r="P19" s="43"/>
     </row>
     <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="51"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="12"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1594,34 +1615,34 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="3"/>
-      <c r="N20" s="54" t="s">
+      <c r="N20" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="O20" s="55" t="s">
+      <c r="O20" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="P20" s="51"/>
+      <c r="P20" s="36"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="52"/>
-      <c r="O21" s="53"/>
-      <c r="P21" s="51"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="36"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
+      <c r="A22" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2166,13 +2187,13 @@
       <c r="F5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="33" t="s">
+      <c r="G5" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="26" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="7">
@@ -2191,7 +2212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{766300AC-A23B-439C-94CC-10586ED209F8}">
   <dimension ref="B1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>

</xml_diff>